<commit_message>
Final Neon migration, updated tariffs, and handover-ready version
</commit_message>
<xml_diff>
--- a/Tarrifs_repairs.xlsx
+++ b/Tarrifs_repairs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Priyesh\repair_portal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Priyesh\alliance_portal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8BDDBA-8EA3-4C35-8D00-1AFCF3B57A1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF37BBCD-0D77-4F41-90EE-D1EC49D115DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="260">
   <si>
     <t>Category</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>DESCRIPTION OF REPAIRS</t>
-  </si>
-  <si>
     <t>ROOF</t>
   </si>
   <si>
@@ -306,9 +303,6 @@
     <t>REPLACE TIR CORD 40'</t>
   </si>
   <si>
-    <t>UNNAMED</t>
-  </si>
-  <si>
     <t>REPLACE STEEL VENTILATOR WITH COMPONENETS&amp;INNER VENT COVER PANEL</t>
   </si>
   <si>
@@ -480,9 +474,6 @@
     <t>STRAIGHTEN COMPLETE CROSS-MEMBER/ FORK POCKET SIDE EACH</t>
   </si>
   <si>
-    <t>UNNAMED1</t>
-  </si>
-  <si>
     <t>STRAIGHTEN AND WELD CROSS- MEMBER / FORK-POCKET SIDE/ OUTRIGGER / RAILFIRST 6 IN.</t>
   </si>
   <si>
@@ -678,9 +669,6 @@
     <t xml:space="preserve">12"  X  6"   </t>
   </si>
   <si>
-    <t xml:space="preserve">EVERY ADDITIONAL PLANK FLOOR                                   </t>
-  </si>
-  <si>
     <t xml:space="preserve">36"  X   6" </t>
   </si>
   <si>
@@ -808,6 +796,15 @@
   </si>
   <si>
     <t>EVERY ADDITIONAL SIDE . (STRAIGHTEN COMPLETE CROSS-MEMBER/ FORK POCKET)</t>
+  </si>
+  <si>
+    <t>PANEL</t>
+  </si>
+  <si>
+    <t>TIR CORD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADDITIONAL PLANK FLOOR                                   </t>
   </si>
 </sst>
 </file>
@@ -1205,8 +1202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A204" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I218" sqref="I218"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,18 +1223,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1">
         <v>4037.33</v>
@@ -1245,10 +1242,10 @@
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1">
         <v>4335.41</v>
@@ -1256,10 +1253,10 @@
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1">
         <v>273.24</v>
@@ -1267,10 +1264,10 @@
     </row>
     <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D5" s="1">
         <v>455.4</v>
@@ -1278,13 +1275,13 @@
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D6" s="1">
         <v>288.14</v>
@@ -1292,13 +1289,13 @@
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C7" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D7" s="1">
         <v>132.47999999999999</v>
@@ -1306,13 +1303,13 @@
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D8" s="1">
         <v>140.76</v>
@@ -1320,13 +1317,13 @@
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D9" s="1">
         <v>215.28</v>
@@ -1334,13 +1331,13 @@
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C10" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D10" s="1">
         <v>761.76</v>
@@ -1348,13 +1345,13 @@
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C11" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D11" s="1">
         <v>1506.96</v>
@@ -1362,13 +1359,13 @@
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C12" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D12" s="1">
         <v>132.47999999999999</v>
@@ -1376,13 +1373,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D13" s="1">
         <v>33.119999999999997</v>
@@ -1390,13 +1387,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C14" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D14" s="1">
         <v>66.239999999999995</v>
@@ -1404,13 +1401,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C15" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D15" s="1">
         <v>99.36</v>
@@ -1418,13 +1415,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C16" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D16" s="1">
         <v>124.2</v>
@@ -1432,13 +1429,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C17" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D17" s="1">
         <v>149.04</v>
@@ -1446,13 +1443,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C18" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D18" s="1">
         <v>207</v>
@@ -1460,13 +1457,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C19" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D19" s="1">
         <v>20.7</v>
@@ -1474,10 +1471,10 @@
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="D20" s="1">
         <v>89.42</v>
@@ -1485,10 +1482,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="1">
@@ -1497,10 +1494,10 @@
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D22" s="1">
         <v>4802.3999999999996</v>
@@ -1508,10 +1505,10 @@
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D23" s="1">
         <v>195.41</v>
@@ -1519,10 +1516,10 @@
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D24" s="1">
         <v>49.68</v>
@@ -1530,10 +1527,10 @@
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D25" s="1">
         <v>107.64</v>
@@ -1541,10 +1538,10 @@
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D26" s="1">
         <v>3643.2</v>
@@ -1552,10 +1549,10 @@
     </row>
     <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D27" s="1">
         <v>7779.89</v>
@@ -1563,10 +1560,10 @@
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D28" s="1">
         <v>1490.4</v>
@@ -1574,10 +1571,10 @@
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D29" s="1">
         <v>2215.73</v>
@@ -1585,10 +1582,10 @@
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D30" s="1">
         <v>1768.61</v>
@@ -1596,10 +1593,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D31" s="1">
         <v>76.180000000000007</v>
@@ -1607,10 +1604,10 @@
     </row>
     <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D32" s="1">
         <v>331.2</v>
@@ -1618,10 +1615,10 @@
     </row>
     <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="1">
@@ -1630,10 +1627,10 @@
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D34" s="1">
         <v>347.76</v>
@@ -1641,10 +1638,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="1">
@@ -1653,10 +1650,10 @@
     </row>
     <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D36" s="1">
         <v>2811.89</v>
@@ -1664,10 +1661,10 @@
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D37" s="1">
         <v>1319.04</v>
@@ -1675,10 +1672,10 @@
     </row>
     <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D38" s="1">
         <v>158.97999999999999</v>
@@ -1686,10 +1683,10 @@
     </row>
     <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C39" s="6"/>
       <c r="D39" s="1">
@@ -1698,10 +1695,10 @@
     </row>
     <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D40" s="1">
         <v>337.82</v>
@@ -1709,13 +1706,13 @@
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C41" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D41" s="1">
         <v>57.96</v>
@@ -1723,13 +1720,13 @@
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C42" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D42" s="1">
         <v>82.2</v>
@@ -1737,13 +1734,13 @@
     </row>
     <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C43" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D43" s="1">
         <v>107.64</v>
@@ -1751,13 +1748,13 @@
     </row>
     <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C44" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D44" s="1">
         <v>193.2</v>
@@ -1765,10 +1762,10 @@
     </row>
     <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C45" s="6"/>
       <c r="D45" s="1">
@@ -1777,10 +1774,10 @@
     </row>
     <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D46" s="1">
         <v>4554</v>
@@ -1788,10 +1785,10 @@
     </row>
     <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D47" s="1">
         <v>9618.0499999999993</v>
@@ -1799,10 +1796,10 @@
     </row>
     <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D48" s="1">
         <v>2583.36</v>
@@ -1810,10 +1807,10 @@
     </row>
     <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D49" s="1">
         <v>2672.78</v>
@@ -1821,10 +1818,10 @@
     </row>
     <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D50" s="1">
         <v>476.93</v>
@@ -1832,10 +1829,10 @@
     </row>
     <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C51" s="6"/>
       <c r="D51" s="1">
@@ -1844,10 +1841,10 @@
     </row>
     <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D52" s="1">
         <v>2980.8</v>
@@ -1855,10 +1852,10 @@
     </row>
     <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D53" s="1">
         <v>1490.4</v>
@@ -1866,10 +1863,10 @@
     </row>
     <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D54" s="1">
         <v>1569.89</v>
@@ -1877,13 +1874,13 @@
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C55" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D55" s="1">
         <v>268.27</v>
@@ -1891,13 +1888,13 @@
     </row>
     <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C56" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D56" s="1">
         <v>188.78</v>
@@ -1905,10 +1902,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C57" s="6"/>
       <c r="D57" s="1">
@@ -1917,13 +1914,13 @@
     </row>
     <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C58" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D58" s="1">
         <v>66.239999999999995</v>
@@ -1931,13 +1928,13 @@
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C59" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D59" s="1">
         <v>99.36</v>
@@ -1945,13 +1942,13 @@
     </row>
     <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C60" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D60" s="1">
         <v>198.72</v>
@@ -1959,13 +1956,13 @@
     </row>
     <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C61" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D61" s="1">
         <v>264.95999999999998</v>
@@ -1973,10 +1970,10 @@
     </row>
     <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C62" s="6"/>
       <c r="D62" s="1">
@@ -1985,10 +1982,10 @@
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D63" s="1">
         <v>82.8</v>
@@ -1996,10 +1993,10 @@
     </row>
     <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C64" s="6"/>
       <c r="D64" s="1">
@@ -2008,10 +2005,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D65" s="1">
         <v>6789.6</v>
@@ -2019,10 +2016,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D66" s="1">
         <v>7203.6</v>
@@ -2030,10 +2027,10 @@
     </row>
     <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D67" s="1">
         <v>3030.48</v>
@@ -2041,10 +2038,10 @@
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D68" s="1">
         <v>434.7</v>
@@ -2052,10 +2049,10 @@
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C69" s="6"/>
       <c r="D69" s="1">
@@ -2064,10 +2061,10 @@
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D70" s="1">
         <v>178.85</v>
@@ -2075,10 +2072,10 @@
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C71" s="6"/>
       <c r="D71" s="1">
@@ -2087,10 +2084,10 @@
     </row>
     <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D72" s="1">
         <v>82.8</v>
@@ -2098,10 +2095,10 @@
     </row>
     <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C73" s="6"/>
       <c r="D73" s="1">
@@ -2110,10 +2107,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D74" s="1">
         <v>69.55</v>
@@ -2121,10 +2118,10 @@
     </row>
     <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C75" s="6"/>
       <c r="D75" s="1">
@@ -2133,10 +2130,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D76" s="1">
         <v>463.68</v>
@@ -2144,10 +2141,10 @@
     </row>
     <row r="77" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D77" s="1">
         <v>8485.34</v>
@@ -2155,10 +2152,10 @@
     </row>
     <row r="78" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D78" s="1">
         <v>3588</v>
@@ -2166,10 +2163,10 @@
     </row>
     <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D79" s="1">
         <v>182.16</v>
@@ -2177,10 +2174,10 @@
     </row>
     <row r="80" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D80" s="1">
         <v>745.2</v>
@@ -2188,10 +2185,10 @@
     </row>
     <row r="81" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D81" s="1">
         <v>238.46</v>
@@ -2199,10 +2196,10 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D82" s="1">
         <v>414</v>
@@ -2210,10 +2207,10 @@
     </row>
     <row r="83" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D83" s="1">
         <v>2260.44</v>
@@ -2221,10 +2218,10 @@
     </row>
     <row r="84" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="D84" s="1">
         <v>728.64</v>
@@ -2232,10 +2229,10 @@
     </row>
     <row r="85" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D85" s="1">
         <v>139.1</v>
@@ -2243,13 +2240,13 @@
     </row>
     <row r="86" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C86" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D86" s="1">
         <v>124.2</v>
@@ -2257,13 +2254,13 @@
     </row>
     <row r="87" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C87" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D87" s="1">
         <v>248.4</v>
@@ -2271,13 +2268,13 @@
     </row>
     <row r="88" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C88" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D88" s="1">
         <v>364.32</v>
@@ -2285,13 +2282,13 @@
     </row>
     <row r="89" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C89" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D89" s="1">
         <v>480.24</v>
@@ -2299,10 +2296,10 @@
     </row>
     <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D90" s="1">
         <v>66.239999999999995</v>
@@ -2310,10 +2307,10 @@
     </row>
     <row r="91" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D91" s="1">
         <v>24.84</v>
@@ -2321,10 +2318,10 @@
     </row>
     <row r="92" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D92" s="1">
         <v>49.68</v>
@@ -2332,10 +2329,10 @@
     </row>
     <row r="93" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C93" s="6"/>
       <c r="D93" s="1">
@@ -2344,10 +2341,10 @@
     </row>
     <row r="94" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D94" s="1">
         <v>331.2</v>
@@ -2355,10 +2352,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D95" s="1">
         <v>240.12</v>
@@ -2366,10 +2363,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D96" s="1">
         <v>110.4</v>
@@ -2377,10 +2374,10 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D97" s="1">
         <v>41.4</v>
@@ -2388,10 +2385,10 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D98" s="1">
         <v>99.36</v>
@@ -2399,10 +2396,10 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D99" s="1">
         <v>74.52</v>
@@ -2410,10 +2407,10 @@
     </row>
     <row r="100" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D100" s="1">
         <v>152.35</v>
@@ -2421,10 +2418,10 @@
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D101" s="1">
         <v>3785.62</v>
@@ -2432,10 +2429,10 @@
     </row>
     <row r="102" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D102" s="1">
         <v>59.16</v>
@@ -2443,10 +2440,10 @@
     </row>
     <row r="103" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D103" s="1">
         <v>190.44</v>
@@ -2454,10 +2451,10 @@
     </row>
     <row r="104" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D104" s="1">
         <v>223.56</v>
@@ -2465,10 +2462,10 @@
     </row>
     <row r="105" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D105" s="1">
         <v>228.53</v>
@@ -2476,10 +2473,10 @@
     </row>
     <row r="106" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D106" s="1">
         <v>66.239999999999995</v>
@@ -2487,10 +2484,10 @@
     </row>
     <row r="107" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D107" s="1">
         <v>41.4</v>
@@ -2498,10 +2495,10 @@
     </row>
     <row r="108" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D108" s="1">
         <v>59.62</v>
@@ -2509,10 +2506,10 @@
     </row>
     <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D109" s="1">
         <v>41.4</v>
@@ -2520,10 +2517,10 @@
     </row>
     <row r="110" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D110" s="1">
         <v>101.02</v>
@@ -2531,10 +2528,10 @@
     </row>
     <row r="111" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C111" s="6"/>
       <c r="D111" s="1">
@@ -2543,10 +2540,10 @@
     </row>
     <row r="112" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D112" s="1">
         <v>67.900000000000006</v>
@@ -2554,10 +2551,10 @@
     </row>
     <row r="113" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D113" s="1">
         <v>33.119999999999997</v>
@@ -2565,10 +2562,10 @@
     </row>
     <row r="114" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D114" s="1">
         <v>16.559999999999999</v>
@@ -2576,10 +2573,10 @@
     </row>
     <row r="115" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D115" s="1">
         <v>49.68</v>
@@ -2587,10 +2584,10 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D116" s="1">
         <v>314.64</v>
@@ -2598,10 +2595,10 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D117" s="1">
         <v>99.36</v>
@@ -2609,10 +2606,10 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D118" s="1">
         <v>132.47999999999999</v>
@@ -2620,10 +2617,10 @@
     </row>
     <row r="119" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D119" s="1">
         <v>16.559999999999999</v>
@@ -2631,10 +2628,10 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D120" s="1">
         <v>49.68</v>
@@ -2642,10 +2639,10 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D121" s="1">
         <v>41.4</v>
@@ -2653,10 +2650,10 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D122" s="1">
         <v>41.4</v>
@@ -2664,10 +2661,10 @@
     </row>
     <row r="123" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D123" s="1">
         <v>66.239999999999995</v>
@@ -2675,10 +2672,10 @@
     </row>
     <row r="124" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D124" s="1">
         <v>3875.04</v>
@@ -2686,10 +2683,10 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D125" s="1">
         <v>1606.32</v>
@@ -2697,10 +2694,10 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D126" s="1">
         <v>251.71</v>
@@ -2708,10 +2705,10 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D127" s="1">
         <v>1680.72</v>
@@ -2719,10 +2716,10 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D128" s="1">
         <v>1540.85</v>
@@ -2730,10 +2727,10 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D129" s="1">
         <v>11684.74</v>
@@ -2741,10 +2738,10 @@
     </row>
     <row r="130" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D130" s="1">
         <v>370.94</v>
@@ -2752,10 +2749,10 @@
     </row>
     <row r="131" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D131" s="1">
         <v>367.63</v>
@@ -2763,10 +2760,10 @@
     </row>
     <row r="132" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D132" s="1">
         <v>6923.74</v>
@@ -2774,10 +2771,10 @@
     </row>
     <row r="133" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D133" s="1">
         <v>2603.23</v>
@@ -2785,10 +2782,10 @@
     </row>
     <row r="134" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D134" s="1">
         <v>818.06</v>
@@ -2796,10 +2793,10 @@
     </row>
     <row r="135" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D135" s="1">
         <v>354.38</v>
@@ -2807,10 +2804,10 @@
     </row>
     <row r="136" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D136" s="1">
         <v>150.69999999999999</v>
@@ -2818,10 +2815,10 @@
     </row>
     <row r="137" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D137" s="1">
         <v>1589.76</v>
@@ -2829,10 +2826,10 @@
     </row>
     <row r="138" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D138" s="1">
         <v>178.85</v>
@@ -2840,10 +2837,10 @@
     </row>
     <row r="139" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C139" s="6"/>
       <c r="D139" s="1">
@@ -2852,10 +2849,10 @@
     </row>
     <row r="140" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D140" s="1">
         <v>198.72</v>
@@ -2863,10 +2860,10 @@
     </row>
     <row r="141" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C141" s="7"/>
       <c r="D141" s="1">
@@ -2875,10 +2872,10 @@
     </row>
     <row r="142" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>151</v>
+        <v>10</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D142" s="1">
         <v>59.62</v>
@@ -2886,10 +2883,10 @@
     </row>
     <row r="143" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>151</v>
+        <v>10</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C143" s="6"/>
       <c r="D143" s="1">
@@ -2898,10 +2895,10 @@
     </row>
     <row r="144" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>151</v>
+        <v>10</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D144" s="1">
         <v>38.83</v>
@@ -2909,10 +2906,10 @@
     </row>
     <row r="145" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>151</v>
+        <v>10</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C145" s="6"/>
       <c r="D145" s="1">
@@ -2921,10 +2918,10 @@
     </row>
     <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B146" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="D146" s="1">
         <v>119.23</v>
@@ -2932,10 +2929,10 @@
     </row>
     <row r="147" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>151</v>
+        <v>10</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D147" s="1">
         <v>331.2</v>
@@ -2943,10 +2940,10 @@
     </row>
     <row r="148" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D148" s="1">
         <v>39951</v>
@@ -2954,10 +2951,10 @@
     </row>
     <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D149" s="1">
         <v>76992</v>
@@ -2965,13 +2962,13 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C150" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D150" s="1">
         <v>7680</v>
@@ -2979,13 +2976,13 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C151" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D151" s="1">
         <v>3840</v>
@@ -2993,13 +2990,13 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C152" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D152" s="1">
         <v>3146</v>
@@ -3007,13 +3004,13 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C153" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D153" s="1">
         <v>4800</v>
@@ -3021,13 +3018,13 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C154" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D154" s="1">
         <v>5760</v>
@@ -3035,13 +3032,13 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C155" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D155" s="1">
         <v>1888</v>
@@ -3049,10 +3046,10 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D156" s="1">
         <v>662.4</v>
@@ -3060,24 +3057,27 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C157" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D157" s="1">
         <v>463.68</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="B158" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C158" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D158" s="1">
         <v>745.2</v>
@@ -3085,13 +3085,13 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C159" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D159" s="1">
         <v>1208.8800000000001</v>
@@ -3099,13 +3099,13 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>217</v>
+        <v>259</v>
       </c>
       <c r="C160" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D160" s="1">
         <v>190.44</v>
@@ -3113,13 +3113,13 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>217</v>
+        <v>259</v>
       </c>
       <c r="C161" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D161" s="1">
         <v>309.67</v>
@@ -3127,13 +3127,13 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>217</v>
+        <v>259</v>
       </c>
       <c r="C162" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D162" s="1">
         <v>500.11</v>
@@ -3141,10 +3141,10 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D163" s="1">
         <v>122.54</v>
@@ -3152,10 +3152,10 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D164" s="1">
         <v>15.73</v>
@@ -3163,10 +3163,10 @@
     </row>
     <row r="165" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D165" s="1">
         <v>347.76</v>
@@ -3174,10 +3174,10 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D166" s="1">
         <v>33.119999999999997</v>
@@ -3185,10 +3185,10 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D167" s="1">
         <v>66.239999999999995</v>
@@ -3196,10 +3196,10 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D168" s="1">
         <v>248.4</v>
@@ -3207,10 +3207,10 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D169" s="1">
         <v>414</v>
@@ -3218,10 +3218,10 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B170" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="B170" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="D170" s="1">
         <v>414</v>
@@ -3229,10 +3229,10 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D171" s="1">
         <v>840</v>
@@ -3240,10 +3240,10 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D172" s="1">
         <v>1800</v>
@@ -3251,10 +3251,10 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D173" s="1">
         <v>3600</v>
@@ -3262,10 +3262,10 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C174" s="6"/>
       <c r="D174" s="1">
@@ -3274,10 +3274,10 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D175" s="1">
         <v>69.55</v>
@@ -3285,10 +3285,10 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D176" s="1">
         <v>33.119999999999997</v>
@@ -3296,10 +3296,10 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D177" s="1">
         <v>218.59</v>
@@ -3307,10 +3307,10 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D178" s="1">
         <v>207</v>
@@ -3318,10 +3318,10 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D179" s="1">
         <v>149.04</v>
@@ -3329,10 +3329,10 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D180" s="1">
         <v>24.84</v>
@@ -3340,10 +3340,10 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D181" s="1">
         <v>33.119999999999997</v>
@@ -3351,10 +3351,10 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D182" s="1">
         <v>49.68</v>
@@ -3362,10 +3362,10 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D183" s="1">
         <v>33.119999999999997</v>
@@ -3373,10 +3373,10 @@
     </row>
     <row r="184" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D184" s="1">
         <v>38.83</v>
@@ -3384,10 +3384,10 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D185" s="1">
         <v>33.119999999999997</v>
@@ -3395,10 +3395,10 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D186" s="1">
         <v>82.8</v>
@@ -3406,10 +3406,10 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D187" s="1">
         <v>89.42</v>
@@ -3417,10 +3417,10 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D188" s="1">
         <v>49.68</v>
@@ -3428,10 +3428,10 @@
     </row>
     <row r="189" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D189" s="1">
         <v>13.25</v>
@@ -3439,10 +3439,10 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D190" s="1">
         <v>69.55</v>
@@ -3450,10 +3450,10 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D191" s="1">
         <v>8.2799999999999994</v>
@@ -3461,10 +3461,10 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D192" s="1">
         <v>0.83</v>
@@ -3472,10 +3472,10 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D193" s="1">
         <v>49.68</v>
@@ -3483,10 +3483,10 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D194" s="1">
         <v>82.8</v>
@@ -3494,10 +3494,10 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D195" s="1">
         <v>89.42</v>
@@ -3505,10 +3505,10 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D196" s="1">
         <v>29.81</v>
@@ -3516,10 +3516,10 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D197" s="1">
         <v>563.04</v>
@@ -3527,10 +3527,10 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C198" s="6"/>
       <c r="D198" s="1">
@@ -3539,10 +3539,10 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D199" s="1">
         <v>66.239999999999995</v>
@@ -3550,10 +3550,10 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D200" s="1">
         <v>8445.6</v>
@@ -3561,10 +3561,10 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D201" s="1">
         <v>15360</v>
@@ -3572,10 +3572,10 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D202" s="1">
         <v>51.34</v>
@@ -3583,13 +3583,13 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C203" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D203" s="1">
         <v>69.55</v>
@@ -3597,13 +3597,13 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C204" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D204" s="1">
         <v>149.04</v>
@@ -3611,13 +3611,13 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C205" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D205" s="1">
         <v>387.5</v>
@@ -3625,13 +3625,13 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C206" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D206" s="1">
         <v>705.46</v>
@@ -3639,10 +3639,10 @@
     </row>
     <row r="207" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C207" s="6"/>
       <c r="D207" s="1">
@@ -3651,10 +3651,10 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D208" s="1">
         <v>82.8</v>
@@ -3662,10 +3662,10 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D209" s="1">
         <v>165.6</v>
@@ -3673,10 +3673,10 @@
     </row>
     <row r="210" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D210" s="1">
         <v>1362.64</v>
@@ -3684,10 +3684,10 @@
     </row>
     <row r="211" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D211" s="1">
         <v>26164.799999999999</v>
@@ -3695,10 +3695,10 @@
     </row>
     <row r="212" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D212" s="1">
         <v>6292.8</v>
@@ -3706,10 +3706,10 @@
     </row>
     <row r="213" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D213" s="1">
         <v>5812.56</v>
@@ -3717,10 +3717,10 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D214" s="1">
         <v>69.55</v>
@@ -3728,10 +3728,10 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D215" s="1">
         <v>414</v>
@@ -3739,10 +3739,10 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D216" s="1">
         <v>347.76</v>
@@ -3750,10 +3750,10 @@
     </row>
     <row r="217" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D217" s="1">
         <v>478.58</v>
@@ -3761,10 +3761,10 @@
     </row>
     <row r="218" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D218" s="1">
         <v>761.76</v>
@@ -3772,10 +3772,10 @@
     </row>
     <row r="219" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C219" s="6"/>
       <c r="D219" s="1">
@@ -3784,10 +3784,10 @@
     </row>
     <row r="220" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D220" s="1">
         <v>387.5</v>
@@ -3795,13 +3795,13 @@
     </row>
     <row r="221" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C221" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D221" s="1">
         <v>102.67</v>
@@ -3809,13 +3809,13 @@
     </row>
     <row r="222" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C222" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D222" s="1">
         <v>123.2</v>
@@ -3823,13 +3823,13 @@
     </row>
     <row r="223" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C223" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D223" s="1">
         <v>231.84</v>
@@ -3837,13 +3837,13 @@
     </row>
     <row r="224" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C224" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D224" s="1">
         <v>387.5</v>
@@ -3851,10 +3851,10 @@
     </row>
     <row r="225" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C225" s="6"/>
       <c r="D225" s="1">
@@ -3863,10 +3863,10 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
-        <v>2</v>
+        <v>258</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D226" s="1">
         <v>1490.4</v>
@@ -3874,10 +3874,10 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
-        <v>2</v>
+        <v>258</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D227" s="1">
         <v>2815.2</v>

</xml_diff>